<commit_message>
Story 25: added the bug_report_luxor section to the document bug_report, also created a screenshot folder for bug_report_luxor.
</commit_message>
<xml_diff>
--- a/Homework_4/Bugs_report_Vlad_Dmytrenko.xlsx
+++ b/Homework_4/Bugs_report_Vlad_Dmytrenko.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7215" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs report - Calc" sheetId="1" r:id="rId1"/>
-    <sheet name="Date" sheetId="2" r:id="rId2"/>
+    <sheet name="Bugs report - Luxor" sheetId="3" r:id="rId2"/>
+    <sheet name="Date" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="168">
   <si>
     <t>ID</t>
   </si>
@@ -276,6 +277,258 @@
   </si>
   <si>
     <t>https://dashboard.leantesting.com/en/projects/calculation/38130/bug-tracker#8</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>When you hover over the header logo, the display is incorrect.</t>
+  </si>
+  <si>
+    <t>vladislav</t>
+  </si>
+  <si>
+    <t>A bug, when you hover the mouse over the logo of the cap, the logo changes to a house. The error is indicated in page_incorrect_1.</t>
+  </si>
+  <si>
+    <t>When you hover over the logo of the header, an additional field is displayed with a hint: "link to the title site"</t>
+  </si>
+  <si>
+    <t>1.Open browser.2.open page: https://www.gamehouse.com/games/luxor-quest-for-the-afterlife.3.move the mouse over the logo of the site header.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#1</t>
+  </si>
+  <si>
+    <t>Menu button caps do not match.</t>
+  </si>
+  <si>
+    <t>Missing buttons: "Home", "New", "Top 100", Free", By Category", "Online Games". Invalid capital letter "Warriors". The error is indicated in page_incorrect_2</t>
+  </si>
+  <si>
+    <t>The presence of buttons: "Home", "New", "Top 100", Free", By Category", "Online Games". The correct spelling of "Voiti", as shown in page_correct_2.</t>
+  </si>
+  <si>
+    <t>1.Open browser, 2. Open page: https://www.gamehouse.com/games/luxor-quest-for-the-afterlife, 3. Check header menu buttons visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#2</t>
+  </si>
+  <si>
+    <t>The location "site search" does not meet the requirement.</t>
+  </si>
+  <si>
+    <t>The "site search" field is located in the opposite place from the requirement. The error is indicated in page_incorrect_3.</t>
+  </si>
+  <si>
+    <t>The location "search on the site" is strictly prescribed for the requirement, as shown in page_correct_3.</t>
+  </si>
+  <si>
+    <t>1.Open browser, 2.open the page: https: //www.gamehouse.com/games/luxor-quest-for-the-afterlife., 3.check the "site search" field for the location visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#3</t>
+  </si>
+  <si>
+    <t>The "login" link is not on demand.</t>
+  </si>
+  <si>
+    <t>The "Login" button is not located at the place indicated on request. The error is indicated in page_incorrect_4.</t>
+  </si>
+  <si>
+    <t>The location of the "Login" must be strictly in the place indicated upon request, as shown in page_correct_4.</t>
+  </si>
+  <si>
+    <t>1.Open a browser., 2. Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife"., 3.Сhecking the location of the "howit" link visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#4</t>
+  </si>
+  <si>
+    <t>Links to social networks are not on demand.</t>
+  </si>
+  <si>
+    <t>The location of social network links is not on demand. The error is indicated in page_incorrect_5.</t>
+  </si>
+  <si>
+    <t>The lack of links in the content to social networks, as shown in page_correct_5.</t>
+  </si>
+  <si>
+    <t>1.Open a browser.,2.Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife"., 3.check the content visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#5</t>
+  </si>
+  <si>
+    <t>The background of the game does not meet the requirement.</t>
+  </si>
+  <si>
+    <t>There is no game background as per requirement. The error is indicated in page_incorrect_6.</t>
+  </si>
+  <si>
+    <t>The background of the game must be strictly on demand, as shown in page_correct_6.</t>
+  </si>
+  <si>
+    <t>1.Open a browser., 2. Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife".,3 check the background of the game visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#6</t>
+  </si>
+  <si>
+    <t>The logo for downloading the game does not match.</t>
+  </si>
+  <si>
+    <t>The logo for downloading the game does not meet the requirement. The error is indicated in page_incorrect_7.</t>
+  </si>
+  <si>
+    <t>Availability of logo as per requirement, as shown in page_correct_7.</t>
+  </si>
+  <si>
+    <t>1.Open a browser., 2.Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife"., 3.check the logo for downloading the game visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#7</t>
+  </si>
+  <si>
+    <t>Missing block "game details".</t>
+  </si>
+  <si>
+    <t>Missing: "game name", "Tags", "Publisher", "download button". The error is indicated in page_incorrect_8.</t>
+  </si>
+  <si>
+    <t>Availability: "game name", "Tags", "Publisher", "download button" as per requirement, as shown in page_correct_8.</t>
+  </si>
+  <si>
+    <t>1.Open a browser., 2.Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife".,3.check the block "game details" visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#8</t>
+  </si>
+  <si>
+    <t>Missing download file size.</t>
+  </si>
+  <si>
+    <t>the presence of the file size of the game to download. The error is indicated in page_incorrect_9.</t>
+  </si>
+  <si>
+    <t>The presence of the file size of the game to download as required, as shown in page_correct_9.</t>
+  </si>
+  <si>
+    <t>1.Open a browser., 2.Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife".</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#9</t>
+  </si>
+  <si>
+    <t>Pictures of the game do not match.</t>
+  </si>
+  <si>
+    <t>There are no game pictures as per requirement. The error is indicated in page_incorrect_10.</t>
+  </si>
+  <si>
+    <t>Availability of game pictures as per requirement, as shown in page_correct_10.</t>
+  </si>
+  <si>
+    <t>1.Open a browser.,2.Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife".</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#10</t>
+  </si>
+  <si>
+    <t>The location of the quick return button is up.</t>
+  </si>
+  <si>
+    <t>The location of the "quick return to top" button is not in the specified location as per the requirement. The error is indicated in page_incorrect_11.</t>
+  </si>
+  <si>
+    <t>Existence of the button of "fast return to top" according to requirement, as shown in page_correct_11.</t>
+  </si>
+  <si>
+    <t>1.Open a browser., 2.Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife"., 3.check the button "quick return to the top" visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#11</t>
+  </si>
+  <si>
+    <t>Lack of reviews block.</t>
+  </si>
+  <si>
+    <t>block "reviews" lack. The error is indicated in page_incorrect_12.</t>
+  </si>
+  <si>
+    <t>the presence of the block "reviews" as per the requirement, as shown in page_correct_12.</t>
+  </si>
+  <si>
+    <t>1.Open a browser., 2.Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife"., 3.check the presence of the block "reviews" visually</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#12</t>
+  </si>
+  <si>
+    <t>Unnecessary Recommended Games Block</t>
+  </si>
+  <si>
+    <t>The presence of the block "recommended games" does not meet the requirement. The error is indicated in page_incorrect_13.</t>
+  </si>
+  <si>
+    <t>The absence of the block "recommended games" does not meet the requirement, as shown in page_correct_13.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#13</t>
+  </si>
+  <si>
+    <t>Lack of links in the footer.</t>
+  </si>
+  <si>
+    <t>Lack of links in the footer: "Support", "Developers", "Switch Version", "Sign Up". The error is indicated in page_incorrect_14.</t>
+  </si>
+  <si>
+    <t>The presence of links in the footer: "Support", "Developers", "Switch Version", "Sign Up" according to the requirement, as shown in page_correct_14.</t>
+  </si>
+  <si>
+    <t>1.Open a browser.,2. Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife".,3. Check for links in the footer visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#14</t>
+  </si>
+  <si>
+    <t>The location of the links in the footer.</t>
+  </si>
+  <si>
+    <t>The links in the footer do not meet the requirement. The error is indicated in page_incorrect_15.</t>
+  </si>
+  <si>
+    <t>The location of the link in the footer matches the requirement, as shown in page_correct_15.</t>
+  </si>
+  <si>
+    <t>1.Open a browser.,2.Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife"., 3.checking the location of links in the footer visually.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#15</t>
+  </si>
+  <si>
+    <t>Scaling link headers</t>
+  </si>
+  <si>
+    <t>Scaling link caps do not meet the requirement. The error is indicated in page_incorrect_16.</t>
+  </si>
+  <si>
+    <t>Scaling link caps as per requirement, as shown in page_correct_16.</t>
+  </si>
+  <si>
+    <t>1.Open a browser., 2.Open page: "https://www.gamehouse.com/games/luxor-quest-for-the-afterlife"., 3.Open a responsive design with a resolution of 768 * 1024 in the browser.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#16</t>
   </si>
 </sst>
 </file>
@@ -315,7 +568,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -396,13 +649,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -428,9 +718,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -466,6 +753,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
@@ -750,9 +1048,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,66 +1068,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -870,16 +1169,16 @@
       </c>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
-      <c r="Q2" s="17">
+      <c r="Q2" s="16">
         <v>43726.78125</v>
       </c>
-      <c r="R2" s="18"/>
-      <c r="S2" s="19" t="s">
+      <c r="R2" s="17"/>
+      <c r="S2" s="18" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -906,7 +1205,7 @@
       <c r="I3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="13"/>
       <c r="K3" s="4" t="s">
         <v>51</v>
       </c>
@@ -919,18 +1218,18 @@
       <c r="N3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="13">
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="12">
         <v>43726.849305555559</v>
       </c>
-      <c r="R3" s="14"/>
-      <c r="S3" s="15" t="s">
+      <c r="R3" s="13"/>
+      <c r="S3" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -957,26 +1256,26 @@
       <c r="I4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="4" t="s">
         <v>55</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="13" t="s">
         <v>57</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="13">
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="12">
         <v>43726.915972222225</v>
       </c>
-      <c r="R4" s="14"/>
-      <c r="S4" s="15" t="s">
+      <c r="R4" s="13"/>
+      <c r="S4" s="14" t="s">
         <v>58</v>
       </c>
       <c r="T4" s="1"/>
@@ -1017,7 +1316,7 @@
       <c r="L5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="13" t="s">
         <v>60</v>
       </c>
       <c r="N5" s="4" t="s">
@@ -1025,11 +1324,11 @@
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="13">
+      <c r="Q5" s="12">
         <v>43726.930555555555</v>
       </c>
       <c r="R5" s="4"/>
-      <c r="S5" s="15" t="s">
+      <c r="S5" s="14" t="s">
         <v>61</v>
       </c>
       <c r="T5" s="3"/>
@@ -1077,11 +1376,11 @@
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="13">
+      <c r="Q6" s="12">
         <v>43726.940972222219</v>
       </c>
       <c r="R6" s="4"/>
-      <c r="S6" s="15" t="s">
+      <c r="S6" s="14" t="s">
         <v>66</v>
       </c>
       <c r="T6" s="3"/>
@@ -1129,11 +1428,11 @@
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="13">
+      <c r="Q7" s="12">
         <v>43726.953472222223</v>
       </c>
       <c r="R7" s="4"/>
-      <c r="S7" s="15" t="s">
+      <c r="S7" s="14" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1180,11 +1479,11 @@
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="13">
+      <c r="Q8" s="12">
         <v>43726.966666666667</v>
       </c>
       <c r="R8" s="4"/>
-      <c r="S8" s="15" t="s">
+      <c r="S8" s="14" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1231,11 +1530,11 @@
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="13">
+      <c r="Q9" s="12">
         <v>43726.972916666666</v>
       </c>
       <c r="R9" s="4"/>
-      <c r="S9" s="15" t="s">
+      <c r="S9" s="14" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1319,10 +1618,972 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:S17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="A1:S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" customWidth="1"/>
+    <col min="13" max="13" width="46.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="16">
+        <v>43729.196527777778</v>
+      </c>
+      <c r="R2" s="7"/>
+      <c r="S2" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="12">
+        <v>43729.20416666667</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="12">
+        <v>43729.208333333336</v>
+      </c>
+      <c r="R4" s="4"/>
+      <c r="S4" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="12">
+        <v>43729.212500000001</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="12">
+        <v>43729.215277777781</v>
+      </c>
+      <c r="R6" s="4"/>
+      <c r="S6" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="12">
+        <v>43729.218055555553</v>
+      </c>
+      <c r="R7" s="4"/>
+      <c r="S7" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="12">
+        <v>43729.224999999999</v>
+      </c>
+      <c r="R8" s="4"/>
+      <c r="S8" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="12">
+        <v>43729.229166666664</v>
+      </c>
+      <c r="R9" s="4"/>
+      <c r="S9" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="12">
+        <v>43729.231249999997</v>
+      </c>
+      <c r="R10" s="4"/>
+      <c r="S10" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="12">
+        <v>43729.231944444444</v>
+      </c>
+      <c r="R11" s="4"/>
+      <c r="S11" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="12">
+        <v>43729.234722222223</v>
+      </c>
+      <c r="R12" s="4"/>
+      <c r="S12" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="12">
+        <v>43729.236111111109</v>
+      </c>
+      <c r="R13" s="4"/>
+      <c r="S13" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" s="5"/>
+      <c r="K14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="28">
+        <v>43729.240972222222</v>
+      </c>
+      <c r="R14" s="5"/>
+      <c r="S14" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="28">
+        <v>43729.243055555555</v>
+      </c>
+      <c r="R15" s="5"/>
+      <c r="S15" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="28">
+        <v>43729.245833333334</v>
+      </c>
+      <c r="R16" s="5"/>
+      <c r="S16" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="28">
+        <v>43729.247916666667</v>
+      </c>
+      <c r="R17" s="5"/>
+      <c r="S17" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1" location="1"/>
+    <hyperlink ref="S3" r:id="rId2" location="2"/>
+    <hyperlink ref="S4" r:id="rId3" location="3"/>
+    <hyperlink ref="S5" r:id="rId4" location="4"/>
+    <hyperlink ref="S6" r:id="rId5" location="5"/>
+    <hyperlink ref="S7" r:id="rId6" location="6"/>
+    <hyperlink ref="S8" r:id="rId7" location="7"/>
+    <hyperlink ref="S9" r:id="rId8" location="8"/>
+    <hyperlink ref="S10" r:id="rId9" location="9"/>
+    <hyperlink ref="S11" r:id="rId10" location="10"/>
+    <hyperlink ref="S12" r:id="rId11" location="11"/>
+    <hyperlink ref="S13" r:id="rId12" location="12"/>
+    <hyperlink ref="S14" r:id="rId13" location="13"/>
+    <hyperlink ref="S15" r:id="rId14" location="14"/>
+    <hyperlink ref="S16" r:id="rId15" location="15"/>
+    <hyperlink ref="S17" r:id="rId16" location="16"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$B$3:$B$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$C$3:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$D$3:$D$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$E$3:$E$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$F$3:$F$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H17</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,10 +2591,11 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1349,11 +2611,14 @@
       <c r="E2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -1369,11 +2634,14 @@
       <c r="E3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="23" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="4" t="s">
         <v>23</v>
@@ -1387,11 +2655,14 @@
       <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="24" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
         <v>24</v>
@@ -1405,11 +2676,14 @@
       <c r="E5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="24" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
         <v>25</v>
@@ -1423,11 +2697,12 @@
       <c r="E6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="24" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="4" t="s">
         <v>26</v>
@@ -1437,9 +2712,10 @@
       <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="24"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="4" t="s">
         <v>27</v>
@@ -1449,9 +2725,10 @@
       <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="24"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
         <v>28</v>
@@ -1459,7 +2736,8 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Story 27: Created a Bugs_report_ListBoxer section.
</commit_message>
<xml_diff>
--- a/Homework_4/Bugs_report_Vlad_Dmytrenko.xlsx
+++ b/Homework_4/Bugs_report_Vlad_Dmytrenko.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7215" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs report - Calc" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs report - Luxor" sheetId="3" r:id="rId2"/>
-    <sheet name="Date" sheetId="2" r:id="rId3"/>
+    <sheet name="Bugs report - ListBoxer" sheetId="4" r:id="rId3"/>
+    <sheet name="Date" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="230">
   <si>
     <t>ID</t>
   </si>
@@ -529,6 +530,192 @@
   </si>
   <si>
     <t>https://dashboard.leantesting.com/en/projects/luxor-web-site/38140/bug-tracker#16</t>
+  </si>
+  <si>
+    <t>Spelling mistake in the "Edit" section.</t>
+  </si>
+  <si>
+    <t>v1.98</t>
+  </si>
+  <si>
+    <t>vladyslav</t>
+  </si>
+  <si>
+    <t>v1.99</t>
+  </si>
+  <si>
+    <t>In the main menu, a menu window with the name "Edjt". The error is indicated in page_incorrect_1.</t>
+  </si>
+  <si>
+    <t>In the main menu of the menu window with the name "Edit".</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#1</t>
+  </si>
+  <si>
+    <t>Incorrect display of the program icon.</t>
+  </si>
+  <si>
+    <t>The program icon does not meet the requirement. The error is indicated in page_incorrect_1.</t>
+  </si>
+  <si>
+    <t>Display the program title icon as required.( page_correct_1.bmp).</t>
+  </si>
+  <si>
+    <t>1.Run the program.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#2</t>
+  </si>
+  <si>
+    <t>The items of the "Edit" drop-down menu are blocked: "Cut", "Copy", "Paste".</t>
+  </si>
+  <si>
+    <t>In the Edit menu, the Cut, Copy, and Paste elements are inactive for use.</t>
+  </si>
+  <si>
+    <t>In the "Edit" menu, the "Cut", "Copy" and "Paste" elements are active.</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer. 2.Select data type Character.3.Enter any text in the text box.4.Select text.5.Go to the “Edjt” menu and select “Cut” or “Copy” or “Paste” (see page_incorrect_3.png).</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#3</t>
+  </si>
+  <si>
+    <t>The application writes empty values.</t>
+  </si>
+  <si>
+    <t>The counter of added entries counted clicks on the button as information fields.</t>
+  </si>
+  <si>
+    <t>The counter of added entries remains zero.</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.2.Click the "Add to list" button any number of times (see page_incorrect_4.png).</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#4</t>
+  </si>
+  <si>
+    <t>Sorting numeric data in a descending list is incorrect.</t>
+  </si>
+  <si>
+    <t>Sort in order: 36, 3518, 287, 2, 287.</t>
+  </si>
+  <si>
+    <t>Sort in order: 3518, 287, 36, 20, 2.</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.2.Select Range: All.3.Select Data Type: Numbers.4.List numbers:287, 2, 36, 20,3518.5.Select Sort: Descending (see page_incorrect_5.png).</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#5</t>
+  </si>
+  <si>
+    <t>Sorting numerical data in a list in ascending order is incorrect.</t>
+  </si>
+  <si>
+    <t>Sort in order: 2, 20, 287, 3518, 36.</t>
+  </si>
+  <si>
+    <t>Sort in order: 2, 20, 36, 287, 3518.</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.2.Select Range: All.3.Select Data Type: Numbers.4.List numbers: 3518, 20, 36, 2, 287.5.Select Sort: Ascending (see page_incorrect_6.png).</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#6</t>
+  </si>
+  <si>
+    <t>The application writes the $ sign.</t>
+  </si>
+  <si>
+    <t>Entries created: $$$, 683 $.</t>
+  </si>
+  <si>
+    <t>An empty list.</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.2.Select Data Type: Character.3.Select Range: All.4.List: $$$, 683 $ (see page_incorrect_7.png).</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#7</t>
+  </si>
+  <si>
+    <t>The Clear List button does not work correctly.</t>
+  </si>
+  <si>
+    <t>The record is not removed from the list.</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.2.Select Data Type: Character.3.Select Range: All.4.Enter any text in the text box.5.Delete the record using the Clear List button (see the pag_incorrect_8.png page).</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#8</t>
+  </si>
+  <si>
+    <t>Application writes values greater than 9999</t>
+  </si>
+  <si>
+    <t>Values are recorded if there is a character before or after a digit greater than 9999.</t>
+  </si>
+  <si>
+    <t>Values are not recorded if there is a character before or after a digit greater than 9999.</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.2.Select Data Type: Character and Numeric.3.Select Range: All.4.Enter in the text box: 99999b, b99999 (see pag_incorrect_9.png).</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#9</t>
+  </si>
+  <si>
+    <t>Incorrect filters in numerical mode (0-100, 101-200, 201-300, 300-9999)</t>
+  </si>
+  <si>
+    <t>Filtering by parameters is available: 0-100, 101-200, 201-300, 300-9999</t>
+  </si>
+  <si>
+    <t>Filtering by parameters is available: 0-100, 101-200, 201-300, 301-9999</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.2.Select Data Type: Numeric.3.Select Range (see pag_incorrect_10.png).</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#10</t>
+  </si>
+  <si>
+    <t>Incorrect operation of the Exit button in the File menu.</t>
+  </si>
+  <si>
+    <t>The application terminates and closes.</t>
+  </si>
+  <si>
+    <t>The application continues to work.</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.2.Create a list of values with any three entries.3.In the File menu, select Exit-No (see pag_incorrect_11.png).4.Launch ListBoxer.5.Create a list of values with any three entries.6.In the File menu, select Exit-Cancel (see pag_increment_12.png).</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#11</t>
+  </si>
+  <si>
+    <t>Incorrect translation of buttons in the dialog box.</t>
+  </si>
+  <si>
+    <t>The names of the buttons are translated into Russian.</t>
+  </si>
+  <si>
+    <t>The button names are translated into the language of the dialog box (English).</t>
+  </si>
+  <si>
+    <t>1.Launch ListBoxer.2.Create a list of values with any three entries.3.In the File menu, select Exit-None (see pag_incorrect_13.png).4.Launch ListBoxer.5.Create a list of values with any three entries.6.In the File menu, select Exit-Cancel (see pag_incorrect_14.png).7.Launch ListBoxer.8.Launch ListBoxer.</t>
+  </si>
+  <si>
+    <t>https://dashboard.leantesting.com/en/projects/listboxer-program/38147/bug-tracker#12</t>
   </si>
 </sst>
 </file>
@@ -692,7 +879,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -764,6 +951,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
@@ -1620,9 +1813,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1" sqref="A1:S1"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2580,10 +2773,770 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="A1:S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="31" customWidth="1"/>
+    <col min="12" max="12" width="32.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="51.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="30">
+        <v>43733.495138888888</v>
+      </c>
+      <c r="R2" s="15"/>
+      <c r="S2" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="29">
+        <v>43733.538194444445</v>
+      </c>
+      <c r="R3" s="11"/>
+      <c r="S3" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="29">
+        <v>43733.539583333331</v>
+      </c>
+      <c r="R4" s="11"/>
+      <c r="S4" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="29">
+        <v>43733.540972222225</v>
+      </c>
+      <c r="R5" s="11"/>
+      <c r="S5" s="14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="29">
+        <v>43733.538888888892</v>
+      </c>
+      <c r="R6" s="11"/>
+      <c r="S6" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="29">
+        <v>43733.540972222225</v>
+      </c>
+      <c r="R7" s="11"/>
+      <c r="S7" s="14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="29">
+        <v>43733.54583333333</v>
+      </c>
+      <c r="R8" s="11"/>
+      <c r="S8" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="29">
+        <v>43733.555555555555</v>
+      </c>
+      <c r="R9" s="11"/>
+      <c r="S9" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="29">
+        <v>43733.556944444441</v>
+      </c>
+      <c r="R10" s="11"/>
+      <c r="S10" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="29">
+        <v>43733.559027777781</v>
+      </c>
+      <c r="R11" s="11"/>
+      <c r="S11" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="29">
+        <v>43733.565972222219</v>
+      </c>
+      <c r="R12" s="11"/>
+      <c r="S12" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="255" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="29">
+        <v>43733.572916666664</v>
+      </c>
+      <c r="R13" s="11"/>
+      <c r="S13" s="14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1" location="1"/>
+    <hyperlink ref="S3" r:id="rId2" location="2"/>
+    <hyperlink ref="S4" r:id="rId3" location="3"/>
+    <hyperlink ref="S5" r:id="rId4" location="4"/>
+    <hyperlink ref="S6" r:id="rId5" location="5"/>
+    <hyperlink ref="S7" r:id="rId6" location="6"/>
+    <hyperlink ref="S8" r:id="rId7" location="7"/>
+    <hyperlink ref="S9" r:id="rId8" location="8"/>
+    <hyperlink ref="S10" r:id="rId9" location="9"/>
+    <hyperlink ref="S11" r:id="rId10" location="10"/>
+    <hyperlink ref="S12" r:id="rId11" location="11"/>
+    <hyperlink ref="S13" r:id="rId12" location="12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$A$3:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$B$3:$B$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$C$3:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$D$3:$D$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$E$3:$E$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$F$3:$F$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2642,7 +3595,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="5" t="s">
+        <v>169</v>
+      </c>
       <c r="B4" s="4" t="s">
         <v>23</v>
       </c>

</xml_diff>